<commit_message>
Updated L19 - changed syntax for table() command
</commit_message>
<xml_diff>
--- a/docs/data/quiz/grades_h19.xlsx
+++ b/docs/data/quiz/grades_h19.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\docs\data\quiz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1BBB670-E1EB-42B6-981D-ADC294F30205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FC78DA-2CBA-4A09-835B-3F335B726171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>